<commit_message>
invoke code dont run
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
   </si>
   <si>
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
@@ -199,6 +196,22 @@
   </si>
   <si>
     <t>Credential_ACMESystem</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Url_SHA1Online</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Url_SHA1Online</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>The url for accessing SHA1 Online.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -537,7 +550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -583,25 +598,25 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2823,8 +2838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2868,27 +2883,37 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>